<commit_message>
Fix erroneous comment in the design_input-xx files.
Related to unif(min,max) comment.
</commit_message>
<xml_diff>
--- a/ert/input/distributions/design_input_ahm.xlsx
+++ b/ert/input/distributions/design_input_ahm.xlsx
@@ -467,7 +467,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">orm (mean, max)
+          <t xml:space="preserve">orm (min, max)
 </t>
         </r>
         <r>
@@ -1376,9 +1376,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>154080</xdr:colOff>
+      <xdr:colOff>153720</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1388,7 +1388,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8118720" cy="7604640"/>
+          <a:ext cx="8124840" cy="7604280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1421,9 +1421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>154080</xdr:colOff>
+      <xdr:colOff>153720</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1433,7 +1433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8118720" cy="7604640"/>
+          <a:ext cx="8124840" cy="7604280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1466,9 +1466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>154080</xdr:colOff>
+      <xdr:colOff>153720</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1478,7 +1478,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8118720" cy="7604640"/>
+          <a:ext cx="8124840" cy="7604280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1516,9 +1516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1528,7 +1528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1561,9 +1561,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1573,7 +1573,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1606,9 +1606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1618,7 +1618,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1651,9 +1651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1663,7 +1663,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1696,9 +1696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1708,7 +1708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1741,9 +1741,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1753,7 +1753,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1786,9 +1786,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1798,7 +1798,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1831,9 +1831,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1843,7 +1843,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1876,9 +1876,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1888,7 +1888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1921,9 +1921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1933,7 +1933,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1966,9 +1966,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4294080</xdr:colOff>
+      <xdr:colOff>4293720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1978,7 +1978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6932880" cy="884880"/>
+          <a:ext cx="6932520" cy="884520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2016,7 +2016,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.13"/>
@@ -2083,10 +2083,10 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.44"/>
@@ -2790,7 +2790,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.22"/>
@@ -3156,7 +3156,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.81"/>
   </cols>
@@ -4536,7 +4536,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>